<commit_message>
rearranged lw, sw instructions
</commit_message>
<xml_diff>
--- a/running_time.xlsx
+++ b/running_time.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Instruction type</t>
   </si>
@@ -74,6 +74,18 @@
   </si>
   <si>
     <t>% improvement</t>
+  </si>
+  <si>
+    <t>Factor</t>
+  </si>
+  <si>
+    <t>% improved</t>
+  </si>
+  <si>
+    <t>Grades</t>
+  </si>
+  <si>
+    <t>#Instructions</t>
   </si>
 </sst>
 </file>
@@ -113,7 +125,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -139,16 +151,64 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G19"/>
+  <dimension ref="A2:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,6 +526,9 @@
     <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" customWidth="1"/>
+    <col min="14" max="14" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
@@ -644,7 +707,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F17">
         <v>31961</v>
       </c>
@@ -652,13 +715,47 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19">
         <f>((F17-F16)/F17)*100</f>
         <v>14.949469666155627</v>
       </c>
       <c r="G19" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L20" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="M20" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="N20" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="K21">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="K22">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="K23">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="K24">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved optimization to 26.8%
Changed `outer` to only check odd numbers other than 2
</commit_message>
<xml_diff>
--- a/running_time.xlsx
+++ b/running_time.xlsx
@@ -516,7 +516,7 @@
   <dimension ref="A2:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,18 +568,18 @@
         <v>1</v>
       </c>
       <c r="B6">
-        <v>4211</v>
+        <v>3285</v>
       </c>
       <c r="D6">
         <f>B6</f>
-        <v>4211</v>
+        <v>3285</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6">
         <f>D6*E6</f>
-        <v>4211</v>
+        <v>3285</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -587,18 +587,18 @@
         <v>2</v>
       </c>
       <c r="B7">
-        <v>298</v>
+        <v>397</v>
       </c>
       <c r="D7">
         <f>B7</f>
-        <v>298</v>
+        <v>397</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7">
         <f>D7*E7</f>
-        <v>298</v>
+        <v>397</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -606,18 +606,18 @@
         <v>3</v>
       </c>
       <c r="B8">
-        <v>1167</v>
+        <v>972</v>
       </c>
       <c r="D8">
         <f>B8</f>
-        <v>1167</v>
+        <v>972</v>
       </c>
       <c r="E8">
         <v>2</v>
       </c>
       <c r="F8">
         <f>D8*E8</f>
-        <v>2334</v>
+        <v>1944</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -625,7 +625,7 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <v>795</v>
+        <v>670</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -633,18 +633,18 @@
         <v>5</v>
       </c>
       <c r="B10">
-        <v>964</v>
+        <v>631</v>
       </c>
       <c r="D10">
         <f>B10-(B14+B15-B9)</f>
-        <v>870</v>
+        <v>527</v>
       </c>
       <c r="E10">
         <v>5</v>
       </c>
       <c r="F10">
         <f>D10*E10</f>
-        <v>4350</v>
+        <v>2635</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -665,18 +665,18 @@
         <v>9</v>
       </c>
       <c r="B14">
-        <v>515</v>
+        <v>417</v>
       </c>
       <c r="D14">
         <f>B14</f>
-        <v>515</v>
+        <v>417</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
       <c r="F14">
         <f>D14*E14</f>
-        <v>1030</v>
+        <v>834</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -684,24 +684,24 @@
         <v>10</v>
       </c>
       <c r="B15">
-        <v>374</v>
+        <v>357</v>
       </c>
       <c r="D15">
         <f>B15</f>
-        <v>374</v>
+        <v>357</v>
       </c>
       <c r="E15">
         <v>40</v>
       </c>
       <c r="F15">
         <f>D15*E15</f>
-        <v>14960</v>
+        <v>14280</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F16" s="4">
         <f>SUM(F6:F15)</f>
-        <v>27183</v>
+        <v>23375</v>
       </c>
       <c r="G16" t="s">
         <v>17</v>
@@ -718,7 +718,7 @@
     <row r="19" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19">
         <f>((F17-F16)/F17)*100</f>
-        <v>14.949469666155627</v>
+        <v>26.863990488407747</v>
       </c>
       <c r="G19" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Added an explanatory comment.
</commit_message>
<xml_diff>
--- a/running_time.xlsx
+++ b/running_time.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Instruction type</t>
   </si>
@@ -74,18 +74,6 @@
   </si>
   <si>
     <t>% improvement</t>
-  </si>
-  <si>
-    <t>Factor</t>
-  </si>
-  <si>
-    <t>% improved</t>
-  </si>
-  <si>
-    <t>Grades</t>
-  </si>
-  <si>
-    <t>#Instructions</t>
   </si>
 </sst>
 </file>
@@ -513,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N24"/>
+  <dimension ref="A2:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,18 +556,18 @@
         <v>1</v>
       </c>
       <c r="B6">
-        <v>3285</v>
+        <v>3383</v>
       </c>
       <c r="D6">
         <f>B6</f>
-        <v>3285</v>
+        <v>3383</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6">
         <f>D6*E6</f>
-        <v>3285</v>
+        <v>3383</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -587,18 +575,18 @@
         <v>2</v>
       </c>
       <c r="B7">
-        <v>397</v>
+        <v>218</v>
       </c>
       <c r="D7">
         <f>B7</f>
-        <v>397</v>
+        <v>218</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7">
         <f>D7*E7</f>
-        <v>397</v>
+        <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -606,18 +594,18 @@
         <v>3</v>
       </c>
       <c r="B8">
-        <v>972</v>
+        <v>833</v>
       </c>
       <c r="D8">
         <f>B8</f>
-        <v>972</v>
+        <v>833</v>
       </c>
       <c r="E8">
         <v>2</v>
       </c>
       <c r="F8">
         <f>D8*E8</f>
-        <v>1944</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -625,7 +613,7 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <v>670</v>
+        <v>500</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -633,18 +621,18 @@
         <v>5</v>
       </c>
       <c r="B10">
-        <v>631</v>
+        <v>512</v>
       </c>
       <c r="D10">
         <f>B10-(B14+B15-B9)</f>
-        <v>527</v>
+        <v>420</v>
       </c>
       <c r="E10">
         <v>5</v>
       </c>
       <c r="F10">
         <f>D10*E10</f>
-        <v>2635</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -665,18 +653,18 @@
         <v>9</v>
       </c>
       <c r="B14">
-        <v>417</v>
+        <v>300</v>
       </c>
       <c r="D14">
         <f>B14</f>
-        <v>417</v>
+        <v>300</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
       <c r="F14">
         <f>D14*E14</f>
-        <v>834</v>
+        <v>600</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -684,24 +672,24 @@
         <v>10</v>
       </c>
       <c r="B15">
-        <v>357</v>
+        <v>292</v>
       </c>
       <c r="D15">
         <f>B15</f>
-        <v>357</v>
+        <v>292</v>
       </c>
       <c r="E15">
         <v>40</v>
       </c>
       <c r="F15">
         <f>D15*E15</f>
-        <v>14280</v>
+        <v>11680</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F16" s="4">
         <f>SUM(F6:F15)</f>
-        <v>23375</v>
+        <v>19647</v>
       </c>
       <c r="G16" t="s">
         <v>17</v>
@@ -718,45 +706,17 @@
     <row r="19" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19">
         <f>((F17-F16)/F17)*100</f>
-        <v>26.863990488407747</v>
+        <v>38.528206251368857</v>
       </c>
       <c r="G19" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="20" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K20" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L20" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="M20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="N20" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="K21">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="K22">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="23" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="K23">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="24" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="K24">
-        <v>70</v>
-      </c>
+      <c r="K20" s="5"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>